<commit_message>
update by spr 20221219
</commit_message>
<xml_diff>
--- a/TB&Offset/TBOffset_ClickTrain_Config.xlsx
+++ b/TB&Offset/TBOffset_ClickTrain_Config.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D055115-7F9A-4B8B-A306-F83022A1FBD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4A18BA-2D6D-466B-8A1E-9DA499095FAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="108">
   <si>
     <t>Amp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -437,6 +437,18 @@
   </si>
   <si>
     <t>@Offset_Variance_Gen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,1,1,1,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9,1.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -808,38 +820,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="8.109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.33203125" style="11" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.77734375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.44140625" style="7" customWidth="1"/>
-    <col min="18" max="18" width="14.44140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="22.125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="19.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.75" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="20.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.375" style="11" customWidth="1"/>
+    <col min="13" max="13" width="16.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.75" style="7" customWidth="1"/>
+    <col min="15" max="15" width="14.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5" style="7" customWidth="1"/>
+    <col min="18" max="18" width="14.5" style="7" customWidth="1"/>
     <col min="19" max="19" width="14" style="7" customWidth="1"/>
-    <col min="20" max="20" width="14.21875" style="13" customWidth="1"/>
+    <col min="20" max="20" width="14.25" style="13" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.33203125" style="16" customWidth="1"/>
+    <col min="22" max="23" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.375" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -916,7 +928,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -993,7 +1005,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>101</v>
       </c>
@@ -1027,8 +1039,8 @@
       <c r="N3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="7">
-        <v>1.5</v>
+      <c r="O3" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>44</v>
@@ -1040,7 +1052,7 @@
         <v>1</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="X3" t="s">
         <v>41</v>
@@ -1049,7 +1061,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>101.1</v>
       </c>
@@ -1105,7 +1117,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>102</v>
       </c>
@@ -1149,7 +1161,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>103</v>
       </c>
@@ -1205,7 +1217,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>104</v>
       </c>
@@ -1261,7 +1273,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>105</v>
       </c>
@@ -1320,7 +1332,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>106</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="X9" t="s">
         <v>18</v>
@@ -1379,7 +1391,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>107</v>
       </c>
@@ -1438,7 +1450,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>108</v>
       </c>
@@ -1488,7 +1500,7 @@
         <v>57</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="X11" t="s">
         <v>28</v>
@@ -1497,7 +1509,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>109</v>
       </c>
@@ -1553,7 +1565,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>121</v>
       </c>
@@ -1611,7 +1623,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>122</v>
       </c>
@@ -1669,7 +1681,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>123</v>
       </c>
@@ -1727,7 +1739,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>124</v>
       </c>
@@ -1785,7 +1797,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>125</v>
       </c>
@@ -1846,7 +1858,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
20220314 click train perception
</commit_message>
<xml_diff>
--- a/TB&Offset/TBOffset_ClickTrain_Config.xlsx
+++ b/TB&Offset/TBOffset_ClickTrain_Config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822029C8-F418-4952-90BB-7486F0A81E8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE9C4D5-7B08-4D71-B1D5-C58090F4397F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="203">
   <si>
     <t>Amp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -631,6 +631,186 @@
   </si>
   <si>
     <t>128</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/02/24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLA_Basic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLA_Tone_Basic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/02/28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5,1,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/03/03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_Oscillation_Tone_Sharp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@TB_Tone_Oscillation_Sharp_Gen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/03/04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Offset_IntegrationWin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@Offset_IntWin_Gen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5,1.5;1.5,0.5;1,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>localChange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>changeICI_Tail_N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>changeICI_Head_N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLA_Offset_Int_4_16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_Basic_4o06_In_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.015,1.015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@TB_Local_ICIChange_Gen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,1.015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/03/06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/03/07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_Basic_4o06_In_4_Insert1_2s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_Basic_4o06_In_4_Insert1_5s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_Basic_4o06_In_4_Insert1_1s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/03/10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_Basic_4o06_In_4_Insert1_0o5s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_Basic_4o06_In_4_Insert1_3s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_Basic_4o06_In_4_Insert1_4s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_Basic_4o06_In_4_Insert_Per_1s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@TB_Insert_N_ICI_Gen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>change_TimePoint</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -707,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -734,6 +914,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1014,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z47"/>
+  <dimension ref="A1:AD64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:A40"/>
+    <sheetView tabSelected="1" topLeftCell="L22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U57" sqref="U57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1207,7 @@
     <col min="2" max="2" width="14.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.109375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="26.109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" style="6" customWidth="1"/>
     <col min="7" max="7" width="19.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.77734375" style="7" customWidth="1"/>
@@ -1041,14 +1222,19 @@
     <col min="18" max="18" width="14.44140625" style="7" customWidth="1"/>
     <col min="19" max="19" width="14" style="7" customWidth="1"/>
     <col min="20" max="20" width="14.21875" style="13" customWidth="1"/>
-    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25" customWidth="1"/>
-    <col min="26" max="26" width="18.33203125" style="16" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" style="7" customWidth="1"/>
+    <col min="22" max="22" width="17.109375" style="7" customWidth="1"/>
+    <col min="23" max="23" width="16.109375" style="7" customWidth="1"/>
+    <col min="24" max="24" width="21.109375" style="7" customWidth="1"/>
+    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.109375" customWidth="1"/>
+    <col min="30" max="30" width="29.6640625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1109,26 +1295,38 @@
       <c r="T1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1189,26 +1387,38 @@
       <c r="T2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Z2" s="15" t="s">
+      <c r="AD2" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>101</v>
       </c>
@@ -1257,14 +1467,14 @@
       <c r="T3" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AB3" t="s">
         <v>40</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AD3" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>102</v>
       </c>
@@ -1292,23 +1502,23 @@
       <c r="L4" s="11">
         <v>2000</v>
       </c>
-      <c r="U4">
+      <c r="Y4">
         <v>3000</v>
       </c>
-      <c r="V4">
+      <c r="Z4">
         <v>500</v>
       </c>
-      <c r="W4">
+      <c r="AA4">
         <v>333</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AB4" t="s">
         <v>19</v>
       </c>
-      <c r="Z4" s="16" t="s">
+      <c r="AD4" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>103</v>
       </c>
@@ -1357,31 +1567,31 @@
       <c r="T5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="X5" t="s">
+      <c r="AB5" t="s">
         <v>18</v>
       </c>
-      <c r="Z5" s="16" t="s">
+      <c r="AD5" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>104</v>
+        <v>103.1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>30</v>
+        <v>162</v>
       </c>
       <c r="C6" s="8">
         <v>97656</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>10</v>
@@ -1396,10 +1606,10 @@
         <v>1000</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="14" t="s">
         <v>51</v>
@@ -1413,16 +1623,16 @@
       <c r="T6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="X6" t="s">
+      <c r="AB6" t="s">
         <v>18</v>
       </c>
-      <c r="Z6" s="16" t="s">
+      <c r="AD6" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>30</v>
@@ -1431,13 +1641,13 @@
         <v>97656</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>10</v>
@@ -1445,43 +1655,40 @@
       <c r="H7" s="6">
         <v>0.5</v>
       </c>
-      <c r="K7" s="9">
-        <v>6000</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>34</v>
+      <c r="L7" s="11">
+        <v>2000</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1000</v>
       </c>
       <c r="N7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="O7" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="Q7" s="7" t="s">
+      <c r="O7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="14">
         <v>0</v>
       </c>
-      <c r="S7" s="7">
+      <c r="S7" s="14">
         <v>0</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="X7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB7" t="s">
         <v>18</v>
       </c>
-      <c r="Z7" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AD7" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>30</v>
@@ -1490,10 +1697,10 @@
         <v>97656</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>24</v>
@@ -1508,16 +1715,16 @@
         <v>6000</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="7" t="s">
-        <v>62</v>
+      <c r="O8" s="7">
+        <v>1.5</v>
       </c>
       <c r="Q8" s="7" t="s">
         <v>51</v>
@@ -1529,18 +1736,18 @@
         <v>0</v>
       </c>
       <c r="T8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD8" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>106</v>
-      </c>
-      <c r="X8" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z8" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>107</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>30</v>
@@ -1549,57 +1756,57 @@
         <v>97656</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="6">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="6">
-        <v>26</v>
+        <v>0.5</v>
       </c>
       <c r="K9" s="9">
         <v>6000</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>89</v>
+        <v>69</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="U9">
-        <v>6000</v>
-      </c>
-      <c r="V9">
-        <v>500</v>
-      </c>
-      <c r="W9">
-        <v>333</v>
-      </c>
-      <c r="X9" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="R9" s="7">
+        <v>0</v>
+      </c>
+      <c r="S9" s="7">
+        <v>0</v>
+      </c>
+      <c r="T9" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB9" t="s">
         <v>18</v>
       </c>
-      <c r="Z9" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AD9" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>30</v>
@@ -1608,229 +1815,231 @@
         <v>97656</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="L10" s="11">
-        <v>2000</v>
-      </c>
-      <c r="M10" s="7">
-        <v>1000</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="O10" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q10" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="R10" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="S10" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="T10" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="X10" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z10" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="6">
+        <v>26</v>
+      </c>
+      <c r="K10" s="9">
+        <v>6000</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y10">
+        <v>6000</v>
+      </c>
+      <c r="Z10">
+        <v>500</v>
+      </c>
+      <c r="AA10">
+        <v>333</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD10" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
-        <v>109</v>
+        <v>107.1</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="C11" s="8">
         <v>97656</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="L11" s="11">
-        <v>2000</v>
-      </c>
-      <c r="M11" s="7">
-        <v>1000</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>47</v>
+        <v>1</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="6">
+        <v>26</v>
+      </c>
+      <c r="K11" s="9">
+        <v>6000</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="R11" s="14">
-        <v>0</v>
-      </c>
-      <c r="S11" s="14">
-        <v>0</v>
-      </c>
-      <c r="T11" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="X11" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y11">
+        <v>6000</v>
+      </c>
+      <c r="Z11">
+        <v>500</v>
+      </c>
+      <c r="AA11">
+        <v>333</v>
+      </c>
+      <c r="AB11" t="s">
         <v>18</v>
       </c>
-      <c r="Z11" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AD11" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C12" s="8">
         <v>97656</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>73</v>
+      <c r="D12" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>58</v>
+      <c r="F12" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="17"/>
-      <c r="L12" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>60</v>
+      <c r="H12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="11">
+        <v>2000</v>
+      </c>
+      <c r="M12" s="7">
+        <v>1000</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="R12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="S12" s="7" t="s">
-        <v>60</v>
+        <v>47</v>
+      </c>
+      <c r="O12" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="S12" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="T12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="X12" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z12" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD12" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C13" s="8">
         <v>97656</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>74</v>
+      <c r="D13" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>65</v>
+        <v>0</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="17"/>
-      <c r="L13" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>60</v>
+      <c r="H13" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="11">
+        <v>2000</v>
+      </c>
+      <c r="M13" s="7">
+        <v>1000</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="Q13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="R13" s="14">
+        <v>0</v>
+      </c>
+      <c r="S13" s="14">
+        <v>0</v>
       </c>
       <c r="T13" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="X13" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z13" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD13" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>57</v>
@@ -1839,10 +2048,10 @@
         <v>97656</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>58</v>
@@ -1856,13 +2065,13 @@
       <c r="I14" s="14"/>
       <c r="J14" s="17"/>
       <c r="L14" s="11" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="M14" s="7" t="s">
         <v>60</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="O14" s="7" t="s">
         <v>62</v>
@@ -1879,16 +2088,16 @@
       <c r="T14" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="X14" t="s">
+      <c r="AB14" t="s">
         <v>64</v>
       </c>
-      <c r="Z14" s="16" t="s">
+      <c r="AD14" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>57</v>
@@ -1897,13 +2106,13 @@
         <v>97656</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>10</v>
@@ -1914,13 +2123,13 @@
       <c r="I15" s="14"/>
       <c r="J15" s="17"/>
       <c r="L15" s="11" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>60</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="O15" s="7" t="s">
         <v>62</v>
@@ -1937,16 +2146,16 @@
       <c r="T15" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="X15" t="s">
+      <c r="AB15" t="s">
         <v>64</v>
       </c>
-      <c r="Z15" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AD15" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>57</v>
@@ -1955,13 +2164,13 @@
         <v>97656</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>10</v>
@@ -1972,42 +2181,39 @@
       <c r="I16" s="14"/>
       <c r="J16" s="17"/>
       <c r="L16" s="11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="M16" s="7" t="s">
         <v>60</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="O16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="P16" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="Q16" s="7" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="R16" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T16" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="X16" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z16" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD16" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>57</v>
@@ -2016,13 +2222,13 @@
         <v>97656</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>10</v>
@@ -2033,7 +2239,7 @@
       <c r="I17" s="14"/>
       <c r="J17" s="17"/>
       <c r="L17" s="11" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="M17" s="7" t="s">
         <v>60</v>
@@ -2056,230 +2262,176 @@
       <c r="T17" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="X17" t="s">
+      <c r="AB17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD17" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>125</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="17"/>
+      <c r="L18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="P18" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="T18" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD18" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>126</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I19" s="14"/>
+      <c r="J19" s="17"/>
+      <c r="L19" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="T19" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB19" t="s">
         <v>18</v>
       </c>
-      <c r="Z17" s="16" t="s">
+      <c r="AD19" s="16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="24"/>
-      <c r="Z19" s="25"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>210.1</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" s="8">
-        <v>97656</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H21" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="L21" s="11">
-        <v>2000</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q21" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="R21" s="7">
-        <v>1</v>
-      </c>
-      <c r="S21" s="7">
-        <v>1</v>
-      </c>
-      <c r="T21" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="X21" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z21" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>210.2</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C22" s="8">
-        <v>97656</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="L22" s="11">
-        <v>2000</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="N22" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="O22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q22" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="R22" s="7">
-        <v>1</v>
-      </c>
-      <c r="S22" s="7">
-        <v>1</v>
-      </c>
-      <c r="T22" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="X22" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z22" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>210.3</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" s="8">
-        <v>97656</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H23" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="L23" s="11">
-        <v>2000</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="O23" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q23" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="R23" s="7">
-        <v>1</v>
-      </c>
-      <c r="S23" s="7">
-        <v>1</v>
-      </c>
-      <c r="T23" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="X23" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z23" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="19"/>
+      <c r="X22" s="19"/>
+      <c r="AD22" s="25"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <v>210.4</v>
+        <v>201</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="C24" s="8">
         <v>97656</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>108</v>
@@ -2287,20 +2439,20 @@
       <c r="H24" s="6">
         <v>0.5</v>
       </c>
-      <c r="L24" s="11">
-        <v>2000</v>
+      <c r="L24" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>118</v>
+        <v>71</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="Q24" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="R24" s="7">
         <v>1</v>
@@ -2311,34 +2463,31 @@
       <c r="T24" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X24" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z24" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD24" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
-        <v>210.5</v>
+        <v>201.1</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="C25" s="8">
         <v>97656</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>108</v>
@@ -2346,20 +2495,20 @@
       <c r="H25" s="6">
         <v>0.5</v>
       </c>
-      <c r="L25" s="11">
-        <v>2000</v>
+      <c r="L25" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>117</v>
+        <v>186</v>
       </c>
       <c r="N25" s="7" t="s">
         <v>118</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="Q25" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="R25" s="7">
         <v>1</v>
@@ -2370,34 +2519,31 @@
       <c r="T25" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X25" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z25" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB25" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD25" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <v>211.1</v>
+        <v>201.2</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>130</v>
+        <v>188</v>
       </c>
       <c r="C26" s="8">
         <v>97656</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>108</v>
@@ -2405,20 +2551,20 @@
       <c r="H26" s="6">
         <v>0.5</v>
       </c>
-      <c r="L26" s="11">
-        <v>2000</v>
+      <c r="L26" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="M26" s="7" t="s">
         <v>117</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>119</v>
+        <v>185</v>
       </c>
       <c r="Q26" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="R26" s="7">
         <v>1</v>
@@ -2429,78 +2575,60 @@
       <c r="T26" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X26" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z26" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD26" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
-        <v>211.2</v>
+        <v>202</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="C27" s="8">
         <v>97656</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>121</v>
+        <v>11</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>108</v>
       </c>
       <c r="H27" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="L27" s="11">
-        <v>2000</v>
+        <v>1</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="N27" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="O27" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q27" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="R27" s="7">
-        <v>1</v>
-      </c>
-      <c r="S27" s="7">
-        <v>1</v>
-      </c>
-      <c r="T27" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="X27" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z27" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="Z27">
+        <v>125</v>
+      </c>
+      <c r="AA27">
+        <v>123.1527</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD27" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
-        <v>211.3</v>
+        <v>210.1</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>130</v>
@@ -2515,7 +2643,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>108</v>
@@ -2530,10 +2658,10 @@
         <v>117</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="Q28" s="7" t="s">
         <v>51</v>
@@ -2547,19 +2675,19 @@
       <c r="T28" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X28" t="s">
+      <c r="AB28" t="s">
         <v>122</v>
       </c>
-      <c r="Y28" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z28" s="16" t="s">
+      <c r="AC28" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD28" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
-        <v>211.4</v>
+        <v>210.2</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>130</v>
@@ -2574,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>108</v>
@@ -2589,10 +2717,10 @@
         <v>117</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="Q29" s="7" t="s">
         <v>51</v>
@@ -2606,19 +2734,19 @@
       <c r="T29" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X29" t="s">
+      <c r="AB29" t="s">
         <v>122</v>
       </c>
-      <c r="Y29" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z29" s="16" t="s">
+      <c r="AC29" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD29" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <v>211.5</v>
+        <v>210.3</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>130</v>
@@ -2633,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>108</v>
@@ -2648,10 +2776,10 @@
         <v>117</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="Q30" s="7" t="s">
         <v>51</v>
@@ -2665,19 +2793,19 @@
       <c r="T30" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X30" t="s">
+      <c r="AB30" t="s">
         <v>122</v>
       </c>
-      <c r="Y30" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z30" s="16" t="s">
+      <c r="AC30" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD30" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
-        <v>212.1</v>
+        <v>210.4</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>130</v>
@@ -2692,7 +2820,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>108</v>
@@ -2707,10 +2835,10 @@
         <v>117</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="O31" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q31" s="7" t="s">
         <v>51</v>
@@ -2724,19 +2852,19 @@
       <c r="T31" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X31" t="s">
+      <c r="AB31" t="s">
         <v>122</v>
       </c>
-      <c r="Y31" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z31" s="16" t="s">
+      <c r="AC31" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD31" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
-        <v>212.2</v>
+        <v>210.5</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>130</v>
@@ -2751,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>108</v>
@@ -2766,10 +2894,10 @@
         <v>117</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="O32" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q32" s="7" t="s">
         <v>51</v>
@@ -2783,19 +2911,19 @@
       <c r="T32" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X32" t="s">
+      <c r="AB32" t="s">
         <v>122</v>
       </c>
-      <c r="Y32" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z32" s="16" t="s">
+      <c r="AC32" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD32" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
-        <v>212.3</v>
+        <v>211.1</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>130</v>
@@ -2810,7 +2938,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>108</v>
@@ -2825,10 +2953,10 @@
         <v>117</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="Q33" s="7" t="s">
         <v>51</v>
@@ -2842,19 +2970,19 @@
       <c r="T33" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X33" t="s">
+      <c r="AB33" t="s">
         <v>122</v>
       </c>
-      <c r="Y33" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z33" s="16" t="s">
+      <c r="AC33" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD33" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
-        <v>212.4</v>
+        <v>211.2</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>130</v>
@@ -2869,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>108</v>
@@ -2884,10 +3012,10 @@
         <v>117</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="O34" s="7" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="Q34" s="7" t="s">
         <v>51</v>
@@ -2901,19 +3029,19 @@
       <c r="T34" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X34" t="s">
+      <c r="AB34" t="s">
         <v>122</v>
       </c>
-      <c r="Y34" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z34" s="16" t="s">
+      <c r="AC34" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD34" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
-        <v>212.5</v>
+        <v>211.3</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>130</v>
@@ -2928,7 +3056,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>108</v>
@@ -2943,10 +3071,10 @@
         <v>117</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="O35" s="7" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="Q35" s="7" t="s">
         <v>51</v>
@@ -2960,19 +3088,19 @@
       <c r="T35" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X35" t="s">
+      <c r="AB35" t="s">
         <v>122</v>
       </c>
-      <c r="Y35" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z35" s="16" t="s">
+      <c r="AC35" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD35" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
-        <v>213.1</v>
+        <v>211.4</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>130</v>
@@ -2987,7 +3115,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>108</v>
@@ -3002,7 +3130,7 @@
         <v>117</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="O36" s="7" t="s">
         <v>119</v>
@@ -3019,19 +3147,19 @@
       <c r="T36" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X36" t="s">
+      <c r="AB36" t="s">
         <v>122</v>
       </c>
-      <c r="Y36" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z36" s="16" t="s">
+      <c r="AC36" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD36" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
-        <v>213.2</v>
+        <v>211.5</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>130</v>
@@ -3046,7 +3174,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>108</v>
@@ -3061,7 +3189,7 @@
         <v>117</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="O37" s="7" t="s">
         <v>119</v>
@@ -3078,19 +3206,19 @@
       <c r="T37" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X37" t="s">
+      <c r="AB37" t="s">
         <v>122</v>
       </c>
-      <c r="Y37" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z37" s="16" t="s">
+      <c r="AC37" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD37" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
-        <v>213.3</v>
+        <v>212.1</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>130</v>
@@ -3105,7 +3233,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>108</v>
@@ -3120,10 +3248,10 @@
         <v>117</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>156</v>
+        <v>71</v>
       </c>
       <c r="O38" s="7" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="Q38" s="7" t="s">
         <v>51</v>
@@ -3137,19 +3265,19 @@
       <c r="T38" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X38" t="s">
+      <c r="AB38" t="s">
         <v>122</v>
       </c>
-      <c r="Y38" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z38" s="16" t="s">
+      <c r="AC38" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD38" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
-        <v>213.4</v>
+        <v>212.2</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>130</v>
@@ -3164,7 +3292,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>108</v>
@@ -3179,10 +3307,10 @@
         <v>117</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>156</v>
+        <v>71</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="Q39" s="7" t="s">
         <v>51</v>
@@ -3196,19 +3324,19 @@
       <c r="T39" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X39" t="s">
+      <c r="AB39" t="s">
         <v>122</v>
       </c>
-      <c r="Y39" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z39" s="16" t="s">
+      <c r="AC39" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD39" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
-        <v>213.5</v>
+        <v>212.3</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>130</v>
@@ -3223,7 +3351,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>108</v>
@@ -3238,10 +3366,10 @@
         <v>117</v>
       </c>
       <c r="N40" s="7" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="O40" s="7" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="Q40" s="7" t="s">
         <v>51</v>
@@ -3255,438 +3383,1434 @@
       <c r="T40" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X40" t="s">
+      <c r="AB40" t="s">
         <v>122</v>
       </c>
-      <c r="Y40" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z40" s="16" t="s">
+      <c r="AC40" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD40" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
-        <v>225</v>
+        <v>212.4</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="C41" s="8">
         <v>97656</v>
       </c>
-      <c r="D41" s="17" t="s">
-        <v>76</v>
+      <c r="D41" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41" s="17" t="s">
-        <v>109</v>
+      <c r="F41" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H41" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="I41" s="14"/>
-      <c r="J41" s="17"/>
-      <c r="L41" s="11" t="s">
-        <v>79</v>
+      <c r="H41" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L41" s="11">
+        <v>2000</v>
       </c>
       <c r="M41" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="O41" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q41" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N41" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="O41" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="P41" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q41" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="R41" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="S41" s="7" t="s">
-        <v>56</v>
+      <c r="R41" s="7">
+        <v>1</v>
+      </c>
+      <c r="S41" s="7">
+        <v>1</v>
       </c>
       <c r="T41" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="X41" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z41" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD41" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
-        <v>225.1</v>
+        <v>212.5</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="C42" s="8">
         <v>97656</v>
       </c>
-      <c r="D42" s="17" t="s">
-        <v>76</v>
+      <c r="D42" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="F42" s="17" t="s">
-        <v>114</v>
+      <c r="F42" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H42" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="I42" s="14"/>
-      <c r="J42" s="17"/>
-      <c r="L42" s="11" t="s">
-        <v>79</v>
+      <c r="H42" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L42" s="11">
+        <v>2000</v>
       </c>
       <c r="M42" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N42" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q42" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N42" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="O42" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="P42" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q42" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="R42" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="S42" s="7" t="s">
-        <v>56</v>
+      <c r="R42" s="7">
+        <v>1</v>
+      </c>
+      <c r="S42" s="7">
+        <v>1</v>
       </c>
       <c r="T42" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="X42" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z42" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD42" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
-        <v>225.2</v>
+        <v>213.1</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="C43" s="8">
         <v>97656</v>
       </c>
-      <c r="D43" s="17" t="s">
-        <v>76</v>
+      <c r="D43" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
-      <c r="F43" s="17" t="s">
-        <v>113</v>
+      <c r="F43" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H43" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="I43" s="14"/>
-      <c r="J43" s="17"/>
-      <c r="L43" s="11" t="s">
-        <v>79</v>
+      <c r="H43" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L43" s="11">
+        <v>2000</v>
       </c>
       <c r="M43" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N43" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="O43" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q43" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N43" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="O43" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="P43" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q43" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="R43" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="S43" s="7" t="s">
-        <v>56</v>
+      <c r="R43" s="7">
+        <v>1</v>
+      </c>
+      <c r="S43" s="7">
+        <v>1</v>
       </c>
       <c r="T43" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="X43" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z43" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD43" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
-        <v>225.3</v>
+        <v>213.2</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="C44" s="8">
         <v>97656</v>
       </c>
-      <c r="D44" s="17" t="s">
-        <v>76</v>
+      <c r="D44" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
-      <c r="F44" s="17" t="s">
-        <v>112</v>
+      <c r="F44" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H44" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="I44" s="14"/>
-      <c r="J44" s="17"/>
-      <c r="L44" s="11" t="s">
-        <v>79</v>
+      <c r="H44" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L44" s="11">
+        <v>2000</v>
       </c>
       <c r="M44" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N44" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="O44" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q44" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N44" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="O44" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="P44" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q44" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="R44" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="S44" s="7" t="s">
-        <v>56</v>
+      <c r="R44" s="7">
+        <v>1</v>
+      </c>
+      <c r="S44" s="7">
+        <v>1</v>
       </c>
       <c r="T44" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="X44" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z44" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD44" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
-        <v>225.4</v>
+        <v>213.3</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="C45" s="8">
         <v>97656</v>
       </c>
-      <c r="D45" s="17" t="s">
-        <v>76</v>
+      <c r="D45" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
-      <c r="F45" s="17" t="s">
-        <v>115</v>
+      <c r="F45" s="6" t="s">
+        <v>153</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H45" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="I45" s="14"/>
-      <c r="J45" s="17"/>
-      <c r="L45" s="11" t="s">
-        <v>79</v>
+      <c r="H45" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L45" s="11">
+        <v>2000</v>
       </c>
       <c r="M45" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N45" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="O45" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q45" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N45" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="O45" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="P45" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q45" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="R45" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="S45" s="7" t="s">
-        <v>56</v>
+      <c r="R45" s="7">
+        <v>1</v>
+      </c>
+      <c r="S45" s="7">
+        <v>1</v>
       </c>
       <c r="T45" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="X45" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z45" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD45" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
-        <v>225.5</v>
+        <v>213.4</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="C46" s="8">
         <v>97656</v>
       </c>
-      <c r="D46" s="17" t="s">
-        <v>76</v>
+      <c r="D46" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
-      <c r="F46" s="17" t="s">
-        <v>116</v>
+      <c r="F46" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H46" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="I46" s="14"/>
-      <c r="J46" s="17"/>
-      <c r="L46" s="11" t="s">
-        <v>79</v>
+      <c r="H46" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L46" s="11">
+        <v>2000</v>
       </c>
       <c r="M46" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N46" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="O46" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q46" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N46" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="O46" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="P46" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q46" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="R46" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="S46" s="7" t="s">
-        <v>56</v>
+      <c r="R46" s="7">
+        <v>1</v>
+      </c>
+      <c r="S46" s="7">
+        <v>1</v>
       </c>
       <c r="T46" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="X46" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z46" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD46" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
-        <v>226</v>
+        <v>213.5</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="C47" s="8">
         <v>97656</v>
       </c>
-      <c r="D47" s="17" t="s">
-        <v>87</v>
+      <c r="D47" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>109</v>
+        <v>1</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H47" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="I47" s="14"/>
-      <c r="J47" s="17"/>
-      <c r="L47" s="11" t="s">
-        <v>79</v>
+      <c r="H47" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L47" s="11">
+        <v>2000</v>
       </c>
       <c r="M47" s="7" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="N47" s="7" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="O47" s="7" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="Q47" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="R47" s="7" t="s">
+      <c r="R47" s="7">
+        <v>1</v>
+      </c>
+      <c r="S47" s="7">
+        <v>1</v>
+      </c>
+      <c r="T47" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD47" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>214</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C48" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H48" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L48" s="11">
+        <v>2000</v>
+      </c>
+      <c r="M48" s="7">
+        <v>1000</v>
+      </c>
+      <c r="N48" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="O48" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q48" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="R48" s="7">
+        <v>1</v>
+      </c>
+      <c r="S48" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="T48" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD48" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>214.1</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H49" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L49" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="M49" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N49" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="O49" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q49" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="R49" s="7">
+        <v>1</v>
+      </c>
+      <c r="S49" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="S47" s="7" t="s">
+      <c r="T49" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD49" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>214.2</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C50" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H50" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L50" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="N50" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="O50" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q50" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R50" s="7">
+        <v>1</v>
+      </c>
+      <c r="S50" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="T47" s="13" t="s">
+      <c r="T50" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD50" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>214.3</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C51" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H51" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L51" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N51" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="O51" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q51" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R51" s="7">
+        <v>1</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="T51" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD51" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:30" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>214.4</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C52" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H52" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L52" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N52" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="O52" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q52" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R52" s="7">
+        <v>1</v>
+      </c>
+      <c r="S52" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="T52" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD52" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>214.5</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H53" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L53" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="M53" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N53" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="O53" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q53" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R53" s="7">
+        <v>1</v>
+      </c>
+      <c r="S53" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="T53" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD53" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>214.6</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C54" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H54" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L54" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N54" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="O54" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q54" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R54" s="7">
+        <v>1</v>
+      </c>
+      <c r="S54" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="T54" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD54" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>214.7</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H55" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L55" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="M55" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N55" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="O55" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q55" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R55" s="7">
+        <v>1</v>
+      </c>
+      <c r="S55" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="T55" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD55" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>215</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C56" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H56" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L56" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="N56" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="O56" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q56" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="R56" s="7">
+        <v>1</v>
+      </c>
+      <c r="S56" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="T56" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="U56" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="V56" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="W56" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="X56" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD56" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>225</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C57" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H57" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I57" s="14"/>
+      <c r="J57" s="17"/>
+      <c r="L57" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M57" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N57" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O57" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P57" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q57" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R57" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="S57" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T57" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD57" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>225.1</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H58" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I58" s="14"/>
+      <c r="J58" s="17"/>
+      <c r="L58" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M58" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N58" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O58" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P58" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q58" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R58" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="S58" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T58" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD58" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>225.2</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H59" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I59" s="14"/>
+      <c r="J59" s="17"/>
+      <c r="L59" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M59" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N59" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O59" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P59" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q59" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R59" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="S59" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T59" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD59" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>225.3</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H60" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I60" s="14"/>
+      <c r="J60" s="17"/>
+      <c r="L60" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M60" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N60" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O60" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P60" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q60" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R60" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="S60" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T60" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD60" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>225.4</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H61" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I61" s="14"/>
+      <c r="J61" s="17"/>
+      <c r="L61" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M61" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N61" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O61" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P61" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q61" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R61" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="S61" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T61" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD61" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>225.5</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H62" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I62" s="14"/>
+      <c r="J62" s="17"/>
+      <c r="L62" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M62" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N62" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O62" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P62" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q62" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R62" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="S62" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T62" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD62" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>226</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" s="8">
+        <v>97656</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H63" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I63" s="14"/>
+      <c r="J63" s="17"/>
+      <c r="L63" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M63" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N63" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O63" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q63" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="R63" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S63" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="T63" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="X47" t="s">
+      <c r="AB63" t="s">
         <v>18</v>
       </c>
-      <c r="Z47" s="16" t="s">
+      <c r="AD63" s="16" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A64" s="17">
+        <v>227</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C64" s="26">
+        <v>97656</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H64" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I64" s="14"/>
+      <c r="J64" s="17"/>
+      <c r="L64" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="M64" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="N64" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="O64" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q64" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="R64" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="S64" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="T64" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="U64" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="V64" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="W64" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD64" s="16" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>